<commit_message>
minor chnages and tracker explanation
</commit_message>
<xml_diff>
--- a/docs/Tracker.xlsx
+++ b/docs/Tracker.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyOwnProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amita\eclipse-workspace\ds-algorithms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAE6D1E-DC93-46D5-8F69-C55E08945483}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22935" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,9 +59,6 @@
     <t>Height of a tree - recursive</t>
   </si>
   <si>
-    <t>Top View of a Tree</t>
-  </si>
-  <si>
     <t>Counting The vallyes - keep current &amp; previous position with a counter which can go +ve or -ve</t>
   </si>
   <si>
@@ -213,9 +209,6 @@
     <t>Insert a node to sorted doubly linked list - check and insert in appropriate place</t>
   </si>
   <si>
-    <t>Reverse a doubly linked list - keep heat as it is, use 3 pointers to reverse. Finally set head.next to null and last pointer to prev to null</t>
-  </si>
-  <si>
     <t>Cookie to be mixed to increase sweetness - use heap, priority queue, keep operation counter increase every time. Finally check that the queue is not empty</t>
   </si>
   <si>
@@ -249,9 +242,6 @@
     <t>Luck Balance - add all the luck, then sort the one with 1 and if more than k substract twice the luck balance</t>
   </si>
   <si>
-    <t>Max - Min unfairness reduction - sort the array, then two index k apart points to mic &amp; max of that subarray. Increment both the index and calculate min unfairness</t>
-  </si>
-  <si>
     <t>Counting Inversion using merge sort - must do merge sort (arr, res, l,r) then merge(arr,res,l,m+1,r) inversion count is invCount+m-i</t>
   </si>
   <si>
@@ -280,12 +270,21 @@
   </si>
   <si>
     <t>Min-Max riddle - this one tricky, use an create right and left next min indexes, then use formula ringht[i]-left[i]-1 to calculate windowSize, then keep collecting max of every window size *****</t>
+  </si>
+  <si>
+    <t>Max - Min unfairness reduction - sort the array, then two index k apart points to min &amp; max of that subarray. Increment both the index and calculate min unfairness</t>
+  </si>
+  <si>
+    <t>Top View of a Tree - breadth first traversal using a queue, keep track of index and if stored skipp</t>
+  </si>
+  <si>
+    <t>Reverse a doubly linked list - keep head as it is, use 3 pointers to reverse. Finally set head.next to null and last pointer to prev to null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +326,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -340,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -373,6 +384,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,21 +675,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="7"/>
-    <col min="2" max="2" width="210.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="210.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -681,399 +698,399 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
         <v>1</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>1</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>1</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
         <v>1</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
-        <v>1</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>1</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
-        <v>1</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
-        <v>1</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
-        <v>1</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
-        <v>1</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
-        <v>1</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
-        <v>1</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>1</v>
       </c>
@@ -1081,185 +1098,185 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="7">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
         <v>1</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>1</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
         <v>1</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>1</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>1</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>1</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>1</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>1</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>1</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>1</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>1</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="9">
-        <v>1</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="9">
-        <v>1</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="10">
-        <v>1</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="8">
-        <v>1</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="10">
-        <v>1</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="9">
-        <v>1</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>1</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>1</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>1</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="10">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
         <v>1</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
         <v>1</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>1</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>1</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>1</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
         <v>1</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>1</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>1</v>
       </c>
@@ -1267,7 +1284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>1</v>
       </c>
@@ -1275,68 +1292,68 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="7">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
         <v>1</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="7">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
         <v>1</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="7">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="14">
         <v>1</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="7">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
         <v>1</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="7">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
         <v>1</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>1</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="13">
         <v>1</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="8">
-        <v>1</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="11">
+        <v>1</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>